<commit_message>
updating code to include new sessions and build out analysis for new varied_size dataset
</commit_message>
<xml_diff>
--- a/ExcelFiles/s3_good_trials_GraspObject_4S_Action.xlsx
+++ b/ExcelFiles/s3_good_trials_GraspObject_4S_Action.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C7D1C-AAD2-48D0-96A2-CB8B3DE6CFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FB94C5-FD91-4AE3-A465-EB384D60DE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="12150" windowHeight="20835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -362,12 +362,12 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
timing analysis and plotting all subjects on same classification plot
</commit_message>
<xml_diff>
--- a/ExcelFiles/s3_good_trials_GraspObject_4S_Action.xlsx
+++ b/ExcelFiles/s3_good_trials_GraspObject_4S_Action.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FB94C5-FD91-4AE3-A465-EB384D60DE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2DA88A-5D6B-415E-9C4F-45AC70C0B487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>2,3,1,2,3,1</t>
+  </si>
+  <si>
+    <t>27,30,36,38</t>
+  </si>
+  <si>
+    <t>19,24,32,28</t>
+  </si>
+  <si>
+    <t>10,16,17,18,20,35</t>
+  </si>
+  <si>
+    <t>2,22,26,28,33,34</t>
   </si>
 </sst>
 </file>
@@ -359,21 +371,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -534,6 +546,49 @@
         <v>6</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20251023</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>